<commit_message>
Minor updates to capitalize 'Lidar' for theme-level in Python tutorials
</commit_message>
<xml_diff>
--- a/processing_code/Redesign_scripts/redesign-FY20-NDS-GitHub-Format.xlsx
+++ b/processing_code/Redesign_scripts/redesign-FY20-NDS-GitHub-Format.xlsx
@@ -5,25 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olearyd/Git/dev-aten/NEON-Data-Skills/processing_code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olearyd/Git/dev-aten/NEON-Data-Skills/processing_code/Redesign_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C591A09-A2D8-FF4A-B34A-241475929C90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C8268FB-B258-D544-8FDD-6B9243EF2AE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site-map" sheetId="1" r:id="rId1"/>
     <sheet name="filepath-map" sheetId="2" r:id="rId2"/>
     <sheet name="ontologies" sheetId="3" r:id="rId3"/>
-    <sheet name="filepath-map-csv" sheetId="4" r:id="rId4"/>
+    <sheet name="redesign-tutorial-filepaths" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="384">
   <si>
     <t>Root</t>
   </si>
@@ -1172,6 +1172,9 @@
   </si>
   <si>
     <t>calc-biomass_py.md</t>
+  </si>
+  <si>
+    <t>tutorials</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1530,7 @@
   </sheetPr>
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
@@ -3410,9 +3413,9 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3443,7 +3446,7 @@
     </row>
     <row r="2" spans="1:6" ht="16">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -3462,8 +3465,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+      <c r="A3" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -3482,8 +3485,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
+      <c r="A4" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -3502,8 +3505,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
+      <c r="A5" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -3522,8 +3525,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="16">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+      <c r="A6" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -3542,8 +3545,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
+      <c r="A7" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -3560,8 +3563,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
+      <c r="A8" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -3580,8 +3583,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
+      <c r="A9" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -3598,8 +3601,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
+      <c r="A10" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
@@ -3618,8 +3621,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
+      <c r="A11" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -3638,8 +3641,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="16">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
+      <c r="A12" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
@@ -3658,8 +3661,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
+      <c r="A13" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
@@ -3678,8 +3681,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="16">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
+      <c r="A14" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
@@ -3698,8 +3701,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
+      <c r="A15" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -3718,8 +3721,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="16">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
+      <c r="A16" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -3738,8 +3741,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="16">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
+      <c r="A17" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -3758,8 +3761,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="16">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
+      <c r="A18" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -3776,8 +3779,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="16">
-      <c r="A19" s="1" t="s">
-        <v>5</v>
+      <c r="A19" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -3796,8 +3799,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="16">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
+      <c r="A20" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -3816,8 +3819,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="16">
-      <c r="A21" s="1" t="s">
-        <v>5</v>
+      <c r="A21" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -3836,8 +3839,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="16">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
+      <c r="A22" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -3856,8 +3859,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="16">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
+      <c r="A23" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -3876,8 +3879,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="16">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
+      <c r="A24" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -3899,8 +3902,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="16">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
+      <c r="A25" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -3919,8 +3922,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="16">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
+      <c r="A26" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -3939,8 +3942,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="16">
-      <c r="A27" s="1" t="s">
-        <v>5</v>
+      <c r="A27" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -3959,8 +3962,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="16">
-      <c r="A28" s="1" t="s">
-        <v>5</v>
+      <c r="A28" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
@@ -3979,8 +3982,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="16">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
+      <c r="A29" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -3999,8 +4002,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="16">
-      <c r="A30" s="1" t="s">
-        <v>5</v>
+      <c r="A30" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
@@ -4019,8 +4022,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="16">
-      <c r="A31" s="1" t="s">
-        <v>5</v>
+      <c r="A31" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
@@ -4039,8 +4042,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="16">
-      <c r="A32" s="1" t="s">
-        <v>5</v>
+      <c r="A32" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
@@ -4059,8 +4062,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="16">
-      <c r="A33" s="1" t="s">
-        <v>5</v>
+      <c r="A33" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>6</v>
@@ -4079,8 +4082,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="16">
-      <c r="A34" s="1" t="s">
-        <v>5</v>
+      <c r="A34" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>6</v>
@@ -4099,8 +4102,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>5</v>
+      <c r="A35" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
@@ -4119,8 +4122,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A36" s="1" t="s">
-        <v>5</v>
+      <c r="A36" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>6</v>
@@ -4139,8 +4142,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
+      <c r="A37" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>6</v>
@@ -4159,8 +4162,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
+      <c r="A38" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>6</v>
@@ -4179,8 +4182,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>5</v>
+      <c r="A39" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
@@ -4197,8 +4200,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="16">
-      <c r="A40" s="1" t="s">
-        <v>5</v>
+      <c r="A40" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
@@ -4215,8 +4218,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>5</v>
+      <c r="A41" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>6</v>
@@ -4233,8 +4236,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="16">
-      <c r="A42" s="1" t="s">
-        <v>5</v>
+      <c r="A42" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>6</v>
@@ -4253,8 +4256,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16">
-      <c r="A43" s="1" t="s">
-        <v>5</v>
+      <c r="A43" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>6</v>
@@ -4273,8 +4276,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="16">
-      <c r="A44" s="1" t="s">
-        <v>5</v>
+      <c r="A44" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>6</v>
@@ -4293,8 +4296,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="16">
-      <c r="A45" s="1" t="s">
-        <v>5</v>
+      <c r="A45" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>6</v>
@@ -4313,8 +4316,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="16">
-      <c r="A46" s="1" t="s">
-        <v>5</v>
+      <c r="A46" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>6</v>
@@ -4333,8 +4336,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="16">
-      <c r="A47" s="1" t="s">
-        <v>5</v>
+      <c r="A47" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>6</v>
@@ -4351,8 +4354,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="16">
-      <c r="A48" s="1" t="s">
-        <v>5</v>
+      <c r="A48" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>6</v>
@@ -4369,8 +4372,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>5</v>
+      <c r="A49" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>6</v>
@@ -4387,8 +4390,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="16">
-      <c r="A50" s="1" t="s">
-        <v>5</v>
+      <c r="A50" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
@@ -4405,8 +4408,8 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="16">
-      <c r="A51" s="1" t="s">
-        <v>5</v>
+      <c r="A51" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>6</v>
@@ -4425,8 +4428,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="16">
-      <c r="A52" s="1" t="s">
-        <v>5</v>
+      <c r="A52" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>6</v>
@@ -4445,8 +4448,8 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="16">
-      <c r="A53" s="1" t="s">
-        <v>5</v>
+      <c r="A53" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>6</v>
@@ -4465,8 +4468,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="16">
-      <c r="A54" s="1" t="s">
-        <v>5</v>
+      <c r="A54" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>6</v>
@@ -4485,8 +4488,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="16">
-      <c r="A55" s="1" t="s">
-        <v>5</v>
+      <c r="A55" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>6</v>
@@ -4505,8 +4508,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="16">
-      <c r="A56" s="1" t="s">
-        <v>5</v>
+      <c r="A56" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>6</v>
@@ -4525,8 +4528,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="16">
-      <c r="A57" s="1" t="s">
-        <v>5</v>
+      <c r="A57" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>6</v>
@@ -4545,8 +4548,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="16">
-      <c r="A58" s="1" t="s">
-        <v>5</v>
+      <c r="A58" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>6</v>
@@ -4565,8 +4568,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="16">
-      <c r="A59" s="1" t="s">
-        <v>5</v>
+      <c r="A59" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>6</v>
@@ -4585,8 +4588,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="16">
-      <c r="A60" s="1" t="s">
-        <v>5</v>
+      <c r="A60" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>6</v>
@@ -4605,8 +4608,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="16">
-      <c r="A61" s="1" t="s">
-        <v>5</v>
+      <c r="A61" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>6</v>
@@ -4625,8 +4628,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="16">
-      <c r="A62" s="1" t="s">
-        <v>5</v>
+      <c r="A62" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>6</v>
@@ -4645,8 +4648,8 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16">
-      <c r="A63" s="1" t="s">
-        <v>5</v>
+      <c r="A63" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>6</v>
@@ -4665,8 +4668,8 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="16">
-      <c r="A64" s="1" t="s">
-        <v>5</v>
+      <c r="A64" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>6</v>
@@ -4685,8 +4688,8 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="16">
-      <c r="A65" s="1" t="s">
-        <v>5</v>
+      <c r="A65" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>6</v>
@@ -4705,8 +4708,8 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="16">
-      <c r="A66" s="1" t="s">
-        <v>5</v>
+      <c r="A66" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>6</v>
@@ -4725,8 +4728,8 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="16">
-      <c r="A67" s="1" t="s">
-        <v>5</v>
+      <c r="A67" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>6</v>
@@ -4745,8 +4748,8 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="16">
-      <c r="A68" s="1" t="s">
-        <v>5</v>
+      <c r="A68" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>6</v>
@@ -4765,8 +4768,8 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="16">
-      <c r="A69" s="1" t="s">
-        <v>5</v>
+      <c r="A69" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>6</v>
@@ -4785,8 +4788,8 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="13">
-      <c r="A70" s="1" t="s">
-        <v>5</v>
+      <c r="A70" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>6</v>
@@ -4805,8 +4808,8 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="16">
-      <c r="A71" s="1" t="s">
-        <v>5</v>
+      <c r="A71" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>6</v>
@@ -4823,8 +4826,8 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="13">
-      <c r="A72" s="1" t="s">
-        <v>5</v>
+      <c r="A72" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>6</v>
@@ -4841,8 +4844,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="13">
-      <c r="A73" s="1" t="s">
-        <v>5</v>
+      <c r="A73" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>6</v>
@@ -4859,8 +4862,8 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="16">
-      <c r="A74" s="1" t="s">
-        <v>5</v>
+      <c r="A74" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>6</v>
@@ -4877,8 +4880,8 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="16">
-      <c r="A75" s="1" t="s">
-        <v>5</v>
+      <c r="A75" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>6</v>
@@ -4898,8 +4901,8 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="13">
-      <c r="A76" s="1" t="s">
-        <v>5</v>
+      <c r="A76" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>6</v>
@@ -4916,8 +4919,8 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="16">
-      <c r="A77" s="1" t="s">
-        <v>5</v>
+      <c r="A77" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>6</v>
@@ -4932,8 +4935,8 @@
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:7" ht="16">
-      <c r="A78" s="1" t="s">
-        <v>5</v>
+      <c r="A78" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>6</v>
@@ -4952,8 +4955,8 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="16">
-      <c r="A79" s="1" t="s">
-        <v>5</v>
+      <c r="A79" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>6</v>
@@ -4972,8 +4975,8 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="16">
-      <c r="A80" s="1" t="s">
-        <v>5</v>
+      <c r="A80" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>6</v>
@@ -4992,8 +4995,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="16">
-      <c r="A81" s="1" t="s">
-        <v>5</v>
+      <c r="A81" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>6</v>
@@ -5012,8 +5015,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="13">
-      <c r="A82" s="1" t="s">
-        <v>5</v>
+      <c r="A82" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>6</v>
@@ -5026,8 +5029,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="13">
-      <c r="A83" s="1" t="s">
-        <v>5</v>
+      <c r="A83" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>6</v>
@@ -5040,8 +5043,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="13">
-      <c r="A84" s="1" t="s">
-        <v>5</v>
+      <c r="A84" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>6</v>
@@ -5060,8 +5063,8 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="13">
-      <c r="A85" s="1" t="s">
-        <v>5</v>
+      <c r="A85" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>6</v>
@@ -5080,8 +5083,8 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="16">
-      <c r="A86" s="1" t="s">
-        <v>5</v>
+      <c r="A86" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>6</v>
@@ -5098,8 +5101,8 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="13">
-      <c r="A87" s="1" t="s">
-        <v>5</v>
+      <c r="A87" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>6</v>
@@ -5114,8 +5117,8 @@
       <c r="F87" s="3"/>
     </row>
     <row r="88" spans="1:6" ht="13">
-      <c r="A88" s="1" t="s">
-        <v>5</v>
+      <c r="A88" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>6</v>
@@ -5128,8 +5131,8 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="13">
-      <c r="A89" s="1" t="s">
-        <v>5</v>
+      <c r="A89" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>6</v>
@@ -5142,8 +5145,8 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="13">
-      <c r="A90" s="1" t="s">
-        <v>5</v>
+      <c r="A90" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>6</v>
@@ -5162,8 +5165,8 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="13">
-      <c r="A91" s="1" t="s">
-        <v>5</v>
+      <c r="A91" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>6</v>
@@ -5182,8 +5185,8 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="16">
-      <c r="A92" s="1" t="s">
-        <v>5</v>
+      <c r="A92" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>6</v>
@@ -5202,8 +5205,8 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="13">
-      <c r="A93" s="1" t="s">
-        <v>5</v>
+      <c r="A93" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>6</v>
@@ -5220,8 +5223,8 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="13">
-      <c r="A94" s="1" t="s">
-        <v>5</v>
+      <c r="A94" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>6</v>
@@ -5240,8 +5243,8 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="16">
-      <c r="A95" s="1" t="s">
-        <v>5</v>
+      <c r="A95" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>6</v>
@@ -5260,8 +5263,8 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="16">
-      <c r="A96" s="1" t="s">
-        <v>5</v>
+      <c r="A96" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>6</v>
@@ -5280,8 +5283,8 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="16">
-      <c r="A97" s="1" t="s">
-        <v>5</v>
+      <c r="A97" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>6</v>
@@ -5300,8 +5303,8 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="16">
-      <c r="A98" s="1" t="s">
-        <v>5</v>
+      <c r="A98" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>6</v>
@@ -5320,8 +5323,8 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="16">
-      <c r="A99" s="1" t="s">
-        <v>5</v>
+      <c r="A99" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>6</v>
@@ -5340,8 +5343,8 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="16">
-      <c r="A100" s="1" t="s">
-        <v>5</v>
+      <c r="A100" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>6</v>
@@ -5360,8 +5363,8 @@
       </c>
     </row>
     <row r="101" spans="1:6" ht="16">
-      <c r="A101" s="1" t="s">
-        <v>5</v>
+      <c r="A101" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>100</v>
@@ -5380,8 +5383,8 @@
       </c>
     </row>
     <row r="102" spans="1:6" ht="16">
-      <c r="A102" s="1" t="s">
-        <v>5</v>
+      <c r="A102" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>100</v>
@@ -5400,8 +5403,8 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="16">
-      <c r="A103" s="1" t="s">
-        <v>5</v>
+      <c r="A103" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>100</v>
@@ -5420,8 +5423,8 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="13">
-      <c r="A104" s="1" t="s">
-        <v>5</v>
+      <c r="A104" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>100</v>
@@ -5440,8 +5443,8 @@
       </c>
     </row>
     <row r="105" spans="1:6" ht="16">
-      <c r="A105" s="1" t="s">
-        <v>5</v>
+      <c r="A105" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>100</v>
@@ -5460,8 +5463,8 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="13">
-      <c r="A106" s="1" t="s">
-        <v>5</v>
+      <c r="A106" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>100</v>
@@ -5473,14 +5476,14 @@
       <c r="F106" s="3"/>
     </row>
     <row r="107" spans="1:6" ht="16">
-      <c r="A107" s="1" t="s">
-        <v>5</v>
+      <c r="A107" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>331</v>
@@ -5493,14 +5496,14 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="16">
-      <c r="A108" s="1" t="s">
-        <v>5</v>
+      <c r="A108" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>110</v>
+      <c r="C108" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>331</v>
@@ -5513,14 +5516,14 @@
       </c>
     </row>
     <row r="109" spans="1:6" ht="16">
-      <c r="A109" s="1" t="s">
-        <v>5</v>
+      <c r="A109" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>110</v>
+      <c r="C109" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>331</v>
@@ -5533,14 +5536,14 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="16">
-      <c r="A110" s="1" t="s">
-        <v>5</v>
+      <c r="A110" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>110</v>
+      <c r="C110" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>331</v>
@@ -5553,8 +5556,8 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="16">
-      <c r="A111" s="1" t="s">
-        <v>5</v>
+      <c r="A111" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>100</v>
@@ -5573,8 +5576,8 @@
       </c>
     </row>
     <row r="112" spans="1:6" ht="16">
-      <c r="A112" s="1" t="s">
-        <v>5</v>
+      <c r="A112" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>100</v>
@@ -5593,8 +5596,8 @@
       </c>
     </row>
     <row r="113" spans="1:6" ht="16">
-      <c r="A113" s="1" t="s">
-        <v>5</v>
+      <c r="A113" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>100</v>
@@ -5613,8 +5616,8 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="16">
-      <c r="A114" s="1" t="s">
-        <v>5</v>
+      <c r="A114" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>100</v>
@@ -5633,8 +5636,8 @@
       </c>
     </row>
     <row r="115" spans="1:6" ht="16">
-      <c r="A115" s="1" t="s">
-        <v>5</v>
+      <c r="A115" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>100</v>
@@ -5653,8 +5656,8 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="16">
-      <c r="A116" s="1" t="s">
-        <v>5</v>
+      <c r="A116" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>100</v>
@@ -5673,8 +5676,8 @@
       </c>
     </row>
     <row r="117" spans="1:6" ht="16">
-      <c r="A117" s="1" t="s">
-        <v>5</v>
+      <c r="A117" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>100</v>
@@ -5693,8 +5696,8 @@
       </c>
     </row>
     <row r="118" spans="1:6" ht="16">
-      <c r="A118" s="1" t="s">
-        <v>5</v>
+      <c r="A118" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>100</v>
@@ -5711,8 +5714,8 @@
       </c>
     </row>
     <row r="119" spans="1:6" ht="16">
-      <c r="A119" s="1" t="s">
-        <v>5</v>
+      <c r="A119" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>100</v>
@@ -5731,8 +5734,8 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="16">
-      <c r="A120" s="1" t="s">
-        <v>5</v>
+      <c r="A120" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>100</v>
@@ -5751,8 +5754,8 @@
       </c>
     </row>
     <row r="121" spans="1:6" ht="16">
-      <c r="A121" s="1" t="s">
-        <v>5</v>
+      <c r="A121" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>100</v>
@@ -5771,8 +5774,8 @@
       </c>
     </row>
     <row r="122" spans="1:6" ht="16">
-      <c r="A122" s="1" t="s">
-        <v>5</v>
+      <c r="A122" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>100</v>
@@ -5791,8 +5794,8 @@
       </c>
     </row>
     <row r="123" spans="1:6" ht="16">
-      <c r="A123" s="1" t="s">
-        <v>5</v>
+      <c r="A123" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>100</v>
@@ -5811,8 +5814,8 @@
       </c>
     </row>
     <row r="124" spans="1:6" ht="16">
-      <c r="A124" s="1" t="s">
-        <v>5</v>
+      <c r="A124" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>100</v>
@@ -5831,8 +5834,8 @@
       </c>
     </row>
     <row r="125" spans="1:6" ht="16">
-      <c r="A125" s="1" t="s">
-        <v>5</v>
+      <c r="A125" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>100</v>
@@ -5851,8 +5854,8 @@
       </c>
     </row>
     <row r="126" spans="1:6" ht="16">
-      <c r="A126" s="1" t="s">
-        <v>5</v>
+      <c r="A126" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>100</v>
@@ -5871,8 +5874,8 @@
       </c>
     </row>
     <row r="127" spans="1:6" ht="16">
-      <c r="A127" s="1" t="s">
-        <v>5</v>
+      <c r="A127" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>100</v>
@@ -5891,14 +5894,14 @@
       </c>
     </row>
     <row r="128" spans="1:6" ht="16">
-      <c r="A128" s="1" t="s">
-        <v>5</v>
+      <c r="A128" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D128" s="14" t="s">
         <v>70</v>
@@ -5911,14 +5914,14 @@
       </c>
     </row>
     <row r="129" spans="1:6" ht="13">
-      <c r="A129" s="1" t="s">
-        <v>5</v>
+      <c r="A129" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>110</v>
+      <c r="C129" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D129" s="14" t="s">
         <v>71</v>
@@ -5931,14 +5934,14 @@
       </c>
     </row>
     <row r="130" spans="1:6" ht="16">
-      <c r="A130" s="1" t="s">
-        <v>5</v>
+      <c r="A130" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>62</v>
@@ -5951,8 +5954,8 @@
       </c>
     </row>
     <row r="131" spans="1:6" ht="16">
-      <c r="A131" s="1" t="s">
-        <v>5</v>
+      <c r="A131" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>100</v>
@@ -5969,8 +5972,8 @@
       </c>
     </row>
     <row r="132" spans="1:6" ht="16">
-      <c r="A132" s="1" t="s">
-        <v>5</v>
+      <c r="A132" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>100</v>
@@ -5989,8 +5992,8 @@
       </c>
     </row>
     <row r="133" spans="1:6" ht="13">
-      <c r="A133" s="1" t="s">
-        <v>5</v>
+      <c r="A133" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>100</v>
@@ -6005,8 +6008,8 @@
       <c r="F133" s="3"/>
     </row>
     <row r="134" spans="1:6" ht="13">
-      <c r="A134" s="1" t="s">
-        <v>5</v>
+      <c r="A134" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>100</v>
@@ -6021,8 +6024,8 @@
       <c r="F134" s="3"/>
     </row>
     <row r="135" spans="1:6" ht="13">
-      <c r="A135" s="1" t="s">
-        <v>5</v>
+      <c r="A135" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>100</v>
@@ -6037,8 +6040,8 @@
       <c r="F135" s="3"/>
     </row>
     <row r="136" spans="1:6" ht="13">
-      <c r="A136" s="1" t="s">
-        <v>5</v>
+      <c r="A136" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>117</v>
@@ -6057,8 +6060,8 @@
       </c>
     </row>
     <row r="137" spans="1:6" ht="16">
-      <c r="A137" s="1" t="s">
-        <v>5</v>
+      <c r="A137" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>117</v>
@@ -6078,7 +6081,7 @@
     </row>
     <row r="138" spans="1:6" ht="16">
       <c r="A138" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>117</v>
@@ -6098,7 +6101,7 @@
     </row>
     <row r="139" spans="1:6" ht="16">
       <c r="A139" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>117</v>
@@ -6118,7 +6121,7 @@
     </row>
     <row r="140" spans="1:6" ht="16">
       <c r="A140" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>117</v>
@@ -6138,7 +6141,7 @@
     </row>
     <row r="141" spans="1:6" ht="16">
       <c r="A141" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>117</v>
@@ -6158,7 +6161,7 @@
     </row>
     <row r="142" spans="1:6" ht="16">
       <c r="A142" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>117</v>
@@ -6178,7 +6181,7 @@
     </row>
     <row r="143" spans="1:6" ht="16">
       <c r="A143" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>117</v>
@@ -6198,7 +6201,7 @@
     </row>
     <row r="144" spans="1:6" ht="16">
       <c r="A144" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>117</v>
@@ -6218,7 +6221,7 @@
     </row>
     <row r="145" spans="1:6" ht="16">
       <c r="A145" s="2" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>117</v>
@@ -6237,8 +6240,8 @@
       </c>
     </row>
     <row r="146" spans="1:6" ht="13">
-      <c r="A146" s="1" t="s">
-        <v>5</v>
+      <c r="A146" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>117</v>
@@ -6255,8 +6258,8 @@
       </c>
     </row>
     <row r="147" spans="1:6" ht="13">
-      <c r="A147" s="1" t="s">
-        <v>5</v>
+      <c r="A147" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>117</v>
@@ -6273,8 +6276,8 @@
       </c>
     </row>
     <row r="148" spans="1:6" ht="16">
-      <c r="A148" s="1" t="s">
-        <v>5</v>
+      <c r="A148" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>117</v>
@@ -6291,8 +6294,8 @@
       </c>
     </row>
     <row r="149" spans="1:6" ht="16">
-      <c r="A149" s="1" t="s">
-        <v>5</v>
+      <c r="A149" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>117</v>
@@ -6309,8 +6312,8 @@
       </c>
     </row>
     <row r="150" spans="1:6" ht="16">
-      <c r="A150" s="1" t="s">
-        <v>5</v>
+      <c r="A150" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>117</v>
@@ -6329,8 +6332,8 @@
       </c>
     </row>
     <row r="151" spans="1:6" ht="13">
-      <c r="A151" s="1" t="s">
-        <v>5</v>
+      <c r="A151" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>117</v>
@@ -6349,8 +6352,8 @@
       </c>
     </row>
     <row r="152" spans="1:6" ht="16">
-      <c r="A152" s="1" t="s">
-        <v>5</v>
+      <c r="A152" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>117</v>
@@ -6369,8 +6372,8 @@
       </c>
     </row>
     <row r="153" spans="1:6" ht="16">
-      <c r="A153" s="1" t="s">
-        <v>5</v>
+      <c r="A153" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>117</v>
@@ -6389,8 +6392,8 @@
       </c>
     </row>
     <row r="154" spans="1:6" ht="13">
-      <c r="A154" s="1" t="s">
-        <v>5</v>
+      <c r="A154" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>117</v>
@@ -7222,8 +7225,8 @@
   <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E97" sqref="E97"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C93" sqref="C93:C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -7256,7 +7259,7 @@
     </row>
     <row r="2" spans="1:6" ht="16">
       <c r="A2" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>6</v>
@@ -7276,7 +7279,7 @@
     </row>
     <row r="3" spans="1:6" ht="13">
       <c r="A3" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -7296,7 +7299,7 @@
     </row>
     <row r="4" spans="1:6" ht="16">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
@@ -7316,7 +7319,7 @@
     </row>
     <row r="5" spans="1:6" ht="16">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>6</v>
@@ -7336,7 +7339,7 @@
     </row>
     <row r="6" spans="1:6" ht="13">
       <c r="A6" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>6</v>
@@ -7356,7 +7359,7 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -7376,7 +7379,7 @@
     </row>
     <row r="8" spans="1:6" ht="16">
       <c r="A8" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -7396,7 +7399,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
@@ -7416,7 +7419,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
@@ -7436,7 +7439,7 @@
     </row>
     <row r="11" spans="1:6" ht="16">
       <c r="A11" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>6</v>
@@ -7456,7 +7459,7 @@
     </row>
     <row r="12" spans="1:6" ht="16">
       <c r="A12" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>6</v>
@@ -7476,7 +7479,7 @@
     </row>
     <row r="13" spans="1:6" ht="16">
       <c r="A13" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>6</v>
@@ -7496,7 +7499,7 @@
     </row>
     <row r="14" spans="1:6" ht="16">
       <c r="A14" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>6</v>
@@ -7516,7 +7519,7 @@
     </row>
     <row r="15" spans="1:6" ht="16">
       <c r="A15" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>6</v>
@@ -7536,7 +7539,7 @@
     </row>
     <row r="16" spans="1:6" ht="16">
       <c r="A16" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>6</v>
@@ -7556,7 +7559,7 @@
     </row>
     <row r="17" spans="1:6" ht="16">
       <c r="A17" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>6</v>
@@ -7576,7 +7579,7 @@
     </row>
     <row r="18" spans="1:6" ht="16">
       <c r="A18" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>6</v>
@@ -7596,7 +7599,7 @@
     </row>
     <row r="19" spans="1:6" ht="16">
       <c r="A19" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>6</v>
@@ -7616,7 +7619,7 @@
     </row>
     <row r="20" spans="1:6" ht="16">
       <c r="A20" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>6</v>
@@ -7636,7 +7639,7 @@
     </row>
     <row r="21" spans="1:6" ht="16">
       <c r="A21" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>6</v>
@@ -7656,7 +7659,7 @@
     </row>
     <row r="22" spans="1:6" ht="16">
       <c r="A22" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>6</v>
@@ -7676,7 +7679,7 @@
     </row>
     <row r="23" spans="1:6" ht="16">
       <c r="A23" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>6</v>
@@ -7696,7 +7699,7 @@
     </row>
     <row r="24" spans="1:6" ht="16">
       <c r="A24" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>6</v>
@@ -7716,7 +7719,7 @@
     </row>
     <row r="25" spans="1:6" ht="16">
       <c r="A25" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>6</v>
@@ -7736,7 +7739,7 @@
     </row>
     <row r="26" spans="1:6" ht="16">
       <c r="A26" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>6</v>
@@ -7756,7 +7759,7 @@
     </row>
     <row r="27" spans="1:6" ht="16">
       <c r="A27" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>6</v>
@@ -7776,7 +7779,7 @@
     </row>
     <row r="28" spans="1:6" ht="16">
       <c r="A28" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>6</v>
@@ -7796,7 +7799,7 @@
     </row>
     <row r="29" spans="1:6" ht="16">
       <c r="A29" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>6</v>
@@ -7816,7 +7819,7 @@
     </row>
     <row r="30" spans="1:6" ht="13">
       <c r="A30" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>6</v>
@@ -7836,7 +7839,7 @@
     </row>
     <row r="31" spans="1:6" ht="16">
       <c r="A31" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>6</v>
@@ -7856,7 +7859,7 @@
     </row>
     <row r="32" spans="1:6" ht="16">
       <c r="A32" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>6</v>
@@ -7876,7 +7879,7 @@
     </row>
     <row r="33" spans="1:6" ht="16">
       <c r="A33" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>6</v>
@@ -7896,7 +7899,7 @@
     </row>
     <row r="34" spans="1:6" ht="16">
       <c r="A34" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>6</v>
@@ -7916,7 +7919,7 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>6</v>
@@ -7936,7 +7939,7 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>6</v>
@@ -7956,7 +7959,7 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>6</v>
@@ -7976,7 +7979,7 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>6</v>
@@ -7996,7 +7999,7 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>6</v>
@@ -8016,7 +8019,7 @@
     </row>
     <row r="40" spans="1:6" ht="13">
       <c r="A40" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>6</v>
@@ -8036,7 +8039,7 @@
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>6</v>
@@ -8056,7 +8059,7 @@
     </row>
     <row r="42" spans="1:6" ht="13">
       <c r="A42" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>6</v>
@@ -8076,7 +8079,7 @@
     </row>
     <row r="43" spans="1:6" ht="16">
       <c r="A43" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>6</v>
@@ -8096,7 +8099,7 @@
     </row>
     <row r="44" spans="1:6" ht="16">
       <c r="A44" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>6</v>
@@ -8116,7 +8119,7 @@
     </row>
     <row r="45" spans="1:6" ht="16">
       <c r="A45" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>6</v>
@@ -8136,7 +8139,7 @@
     </row>
     <row r="46" spans="1:6" ht="16">
       <c r="A46" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>6</v>
@@ -8156,7 +8159,7 @@
     </row>
     <row r="47" spans="1:6" ht="16">
       <c r="A47" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>6</v>
@@ -8175,8 +8178,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="16">
-      <c r="A48" s="2" t="s">
-        <v>5</v>
+      <c r="A48" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>6</v>
@@ -8196,7 +8199,7 @@
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>6</v>
@@ -8216,7 +8219,7 @@
     </row>
     <row r="50" spans="1:6" ht="16">
       <c r="A50" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>6</v>
@@ -8236,7 +8239,7 @@
     </row>
     <row r="51" spans="1:6" ht="16">
       <c r="A51" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>6</v>
@@ -8256,7 +8259,7 @@
     </row>
     <row r="52" spans="1:6" ht="16">
       <c r="A52" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>6</v>
@@ -8276,7 +8279,7 @@
     </row>
     <row r="53" spans="1:6" ht="13">
       <c r="A53" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>6</v>
@@ -8296,7 +8299,7 @@
     </row>
     <row r="54" spans="1:6" ht="16">
       <c r="A54" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>6</v>
@@ -8316,7 +8319,7 @@
     </row>
     <row r="55" spans="1:6" ht="16">
       <c r="A55" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>6</v>
@@ -8336,7 +8339,7 @@
     </row>
     <row r="56" spans="1:6" ht="16">
       <c r="A56" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>6</v>
@@ -8356,7 +8359,7 @@
     </row>
     <row r="57" spans="1:6" ht="16">
       <c r="A57" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>6</v>
@@ -8376,7 +8379,7 @@
     </row>
     <row r="58" spans="1:6" ht="16">
       <c r="A58" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>6</v>
@@ -8396,7 +8399,7 @@
     </row>
     <row r="59" spans="1:6" ht="16">
       <c r="A59" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>6</v>
@@ -8416,7 +8419,7 @@
     </row>
     <row r="60" spans="1:6" ht="16">
       <c r="A60" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>6</v>
@@ -8436,7 +8439,7 @@
     </row>
     <row r="61" spans="1:6" ht="16">
       <c r="A61" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>6</v>
@@ -8456,7 +8459,7 @@
     </row>
     <row r="62" spans="1:6" ht="16">
       <c r="A62" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>6</v>
@@ -8476,7 +8479,7 @@
     </row>
     <row r="63" spans="1:6" ht="16">
       <c r="A63" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>6</v>
@@ -8496,7 +8499,7 @@
     </row>
     <row r="64" spans="1:6" ht="16">
       <c r="A64" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>6</v>
@@ -8516,7 +8519,7 @@
     </row>
     <row r="65" spans="1:8" ht="16">
       <c r="A65" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>6</v>
@@ -8536,7 +8539,7 @@
     </row>
     <row r="66" spans="1:8" ht="16">
       <c r="A66" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>6</v>
@@ -8557,7 +8560,7 @@
     </row>
     <row r="67" spans="1:8" ht="16">
       <c r="A67" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>6</v>
@@ -8577,7 +8580,7 @@
     </row>
     <row r="68" spans="1:8" ht="16">
       <c r="A68" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>6</v>
@@ -8597,7 +8600,7 @@
     </row>
     <row r="69" spans="1:8" ht="16">
       <c r="A69" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>6</v>
@@ -8617,7 +8620,7 @@
     </row>
     <row r="70" spans="1:8" ht="16">
       <c r="A70" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>6</v>
@@ -8637,7 +8640,7 @@
     </row>
     <row r="71" spans="1:8" ht="16">
       <c r="A71" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>6</v>
@@ -8657,7 +8660,7 @@
     </row>
     <row r="72" spans="1:8" ht="16">
       <c r="A72" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>6</v>
@@ -8677,7 +8680,7 @@
     </row>
     <row r="73" spans="1:8" ht="16">
       <c r="A73" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>6</v>
@@ -8697,7 +8700,7 @@
     </row>
     <row r="74" spans="1:8" ht="16">
       <c r="A74" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>6</v>
@@ -8717,7 +8720,7 @@
     </row>
     <row r="75" spans="1:8" ht="16">
       <c r="A75" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>6</v>
@@ -8737,7 +8740,7 @@
     </row>
     <row r="76" spans="1:8" ht="16">
       <c r="A76" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>6</v>
@@ -8757,7 +8760,7 @@
     </row>
     <row r="77" spans="1:8" ht="16">
       <c r="A77" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>100</v>
@@ -8777,7 +8780,7 @@
     </row>
     <row r="78" spans="1:8" ht="16">
       <c r="A78" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>100</v>
@@ -8797,7 +8800,7 @@
     </row>
     <row r="79" spans="1:8" ht="16">
       <c r="A79" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>100</v>
@@ -8817,7 +8820,7 @@
     </row>
     <row r="80" spans="1:8" ht="16">
       <c r="A80" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>100</v>
@@ -8837,7 +8840,7 @@
     </row>
     <row r="81" spans="1:7" ht="16">
       <c r="A81" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>100</v>
@@ -8857,7 +8860,7 @@
     </row>
     <row r="82" spans="1:7" ht="16">
       <c r="A82" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>100</v>
@@ -8877,7 +8880,7 @@
     </row>
     <row r="83" spans="1:7" ht="16">
       <c r="A83" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>100</v>
@@ -8897,7 +8900,7 @@
     </row>
     <row r="84" spans="1:7" ht="16">
       <c r="A84" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>100</v>
@@ -8917,7 +8920,7 @@
     </row>
     <row r="85" spans="1:7" ht="16">
       <c r="A85" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>100</v>
@@ -8937,7 +8940,7 @@
     </row>
     <row r="86" spans="1:7" ht="16">
       <c r="A86" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>100</v>
@@ -8957,7 +8960,7 @@
     </row>
     <row r="87" spans="1:7" ht="16">
       <c r="A87" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>100</v>
@@ -8977,7 +8980,7 @@
     </row>
     <row r="88" spans="1:7" ht="16">
       <c r="A88" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>100</v>
@@ -8997,7 +9000,7 @@
     </row>
     <row r="89" spans="1:7" ht="16">
       <c r="A89" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>100</v>
@@ -9017,7 +9020,7 @@
     </row>
     <row r="90" spans="1:7" ht="16">
       <c r="A90" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>100</v>
@@ -9037,7 +9040,7 @@
     </row>
     <row r="91" spans="1:7" ht="16">
       <c r="A91" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>100</v>
@@ -9057,7 +9060,7 @@
     </row>
     <row r="92" spans="1:7" ht="16">
       <c r="A92" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>100</v>
@@ -9077,13 +9080,13 @@
     </row>
     <row r="93" spans="1:7" ht="16">
       <c r="A93" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>331</v>
@@ -9097,13 +9100,13 @@
     </row>
     <row r="94" spans="1:7" ht="16">
       <c r="A94" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>331</v>
@@ -9117,13 +9120,13 @@
     </row>
     <row r="95" spans="1:7" ht="16">
       <c r="A95" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>110</v>
+      <c r="C95" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>331</v>
@@ -9138,13 +9141,13 @@
     </row>
     <row r="96" spans="1:7" ht="16">
       <c r="A96" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>331</v>
@@ -9158,13 +9161,13 @@
     </row>
     <row r="97" spans="1:6" ht="13">
       <c r="A97" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D97" s="14" t="s">
         <v>71</v>
@@ -9178,13 +9181,13 @@
     </row>
     <row r="98" spans="1:6" ht="16">
       <c r="A98" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>110</v>
+      <c r="C98" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="D98" s="14" t="s">
         <v>70</v>
@@ -9198,13 +9201,13 @@
     </row>
     <row r="99" spans="1:6" ht="16">
       <c r="A99" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>110</v>
+      <c r="C99" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>62</v>
@@ -9218,7 +9221,7 @@
     </row>
     <row r="100" spans="1:6" ht="16">
       <c r="A100" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>100</v>
@@ -9238,7 +9241,7 @@
     </row>
     <row r="101" spans="1:6" ht="13">
       <c r="A101" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>100</v>
@@ -9258,7 +9261,7 @@
     </row>
     <row r="102" spans="1:6" ht="16">
       <c r="A102" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>100</v>
@@ -9278,7 +9281,7 @@
     </row>
     <row r="103" spans="1:6" ht="16">
       <c r="A103" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>100</v>
@@ -9298,7 +9301,7 @@
     </row>
     <row r="104" spans="1:6" ht="16">
       <c r="A104" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>100</v>
@@ -9318,7 +9321,7 @@
     </row>
     <row r="105" spans="1:6" ht="16">
       <c r="A105" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>100</v>
@@ -9337,8 +9340,8 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="16">
-      <c r="A106" s="2" t="s">
-        <v>5</v>
+      <c r="A106" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>117</v>
@@ -9358,7 +9361,7 @@
     </row>
     <row r="107" spans="1:6" ht="16">
       <c r="A107" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>117</v>
@@ -9378,7 +9381,7 @@
     </row>
     <row r="108" spans="1:6" ht="13">
       <c r="A108" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>117</v>
@@ -9398,7 +9401,7 @@
     </row>
     <row r="109" spans="1:6" ht="16">
       <c r="A109" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>117</v>
@@ -9418,7 +9421,7 @@
     </row>
     <row r="110" spans="1:6" ht="16">
       <c r="A110" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>117</v>
@@ -9437,8 +9440,8 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="16">
-      <c r="A111" s="2" t="s">
-        <v>5</v>
+      <c r="A111" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>117</v>
@@ -9458,7 +9461,7 @@
     </row>
     <row r="112" spans="1:6" ht="16">
       <c r="A112" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>117</v>
@@ -9477,8 +9480,8 @@
       </c>
     </row>
     <row r="113" spans="1:6" ht="16">
-      <c r="A113" s="2" t="s">
-        <v>5</v>
+      <c r="A113" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>117</v>
@@ -9497,8 +9500,8 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="16">
-      <c r="A114" s="2" t="s">
-        <v>5</v>
+      <c r="A114" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>117</v>
@@ -9517,8 +9520,8 @@
       </c>
     </row>
     <row r="115" spans="1:6" ht="16">
-      <c r="A115" s="2" t="s">
-        <v>5</v>
+      <c r="A115" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>117</v>
@@ -9537,8 +9540,8 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="16">
-      <c r="A116" s="2" t="s">
-        <v>5</v>
+      <c r="A116" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>117</v>
@@ -9557,8 +9560,8 @@
       </c>
     </row>
     <row r="117" spans="1:6" ht="16">
-      <c r="A117" s="2" t="s">
-        <v>5</v>
+      <c r="A117" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>117</v>
@@ -9577,8 +9580,8 @@
       </c>
     </row>
     <row r="118" spans="1:6" ht="16">
-      <c r="A118" s="2" t="s">
-        <v>5</v>
+      <c r="A118" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>117</v>
@@ -9598,7 +9601,7 @@
     </row>
     <row r="119" spans="1:6" ht="13">
       <c r="A119" s="8" t="s">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>117</v>

</xml_diff>